<commit_message>
Adición de verificaciones de unboarding y única cuenta de deposito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A840D4E6-40A8-4B07-B5BC-30E11A1A3F87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4874E88C-5B3F-4881-9F2D-579F303A8110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Corriente</t>
+  </si>
+  <si>
+    <t>406-785280-05</t>
+  </si>
+  <si>
+    <t>ospciclo4finde</t>
   </si>
 </sst>
 </file>
@@ -553,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -640,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>24</v>
@@ -679,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>36</v>
@@ -696,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>24</v>
@@ -735,7 +741,7 @@
         <v>30</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="R3" s="11">
         <v>120000</v>

</xml_diff>

<commit_message>
Cambios según comentarios de revisor de pull request
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4874E88C-5B3F-4881-9F2D-579F303A8110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F078348F-926C-4C30-9114-6AFD3E6F6FEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>406-785280-05</t>
-  </si>
-  <si>
-    <t>ospciclo4finde</t>
   </si>
 </sst>
 </file>
@@ -560,7 +557,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -646,7 +643,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>24</v>
@@ -702,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Adición de funcionalidad de pago de tarjeta de credito no propia
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/GenerarCodigoQr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F078348F-926C-4C30-9114-6AFD3E6F6FEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2041D6F-B0FF-4BD4-98A2-19C1F29F4C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Corriente</t>
-  </si>
-  <si>
-    <t>406-785280-05</t>
   </si>
 </sst>
 </file>
@@ -556,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -682,7 +679,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>36</v>
@@ -738,7 +735,7 @@
         <v>30</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="R3" s="11">
         <v>120000</v>

</xml_diff>